<commit_message>
Auditoria de calida 28 dic
</commit_message>
<xml_diff>
--- a/Proyectos/2015/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/Calidad/No_conformidades.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -51,19 +51,26 @@
   </si>
   <si>
     <t>Se solicita agregarlo en el próximo reporte</t>
+  </si>
+  <si>
+    <t>No todos los tickets tienen un nombre descriptivo</t>
+  </si>
+  <si>
+    <t>Oriana Osiris</t>
+  </si>
+  <si>
+    <t>Se genera aviso de cambiar el nombre a uno mas descriptivo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="[$$-80A]#,##0.00;[RED]\-[$$-80A]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,32 +92,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -185,7 +166,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,41 +190,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,7 +212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -263,24 +220,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Porcentaje 2" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 1" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 1" xfId="25" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -353,7 +304,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -435,16 +386,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>42366</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>42366</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">

</xml_diff>